<commit_message>
First version: journal manager write to excel
First working version with bugs. The journal manager is writing to the excel file.
</commit_message>
<xml_diff>
--- a/temp text files/trading_journal_color.xlsx
+++ b/temp text files/trading_journal_color.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Cloud Files\TradingTools\trade_journal_project\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Cloud Files\TradingTools\trade_journal_project\temp text files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7986EA2F-BD4B-4516-A1DB-0CFFDBA9C7BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB63A7BF-10D9-4B42-BE4B-8E02DE82F959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trade Log" sheetId="1" r:id="rId1"/>
@@ -322,7 +322,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="27">
+  <fills count="31">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -475,6 +475,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="42">
     <border>
@@ -1074,7 +1098,7 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1189,19 +1213,10 @@
     <xf numFmtId="0" fontId="5" fillId="11" borderId="28" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1231,15 +1246,9 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="13" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1261,6 +1270,51 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="40" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="24" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="27" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="35" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1291,50 +1345,14 @@
     <xf numFmtId="0" fontId="5" fillId="24" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="40" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="24" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="27" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="14" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="15" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="16" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1348,14 +1366,26 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="14" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="15" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="16" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="11" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="17" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="18" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="19" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1366,27 +1396,6 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="13" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="11" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="17" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="18" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="19" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1404,6 +1413,33 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="16" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -1711,37 +1747,37 @@
   <dimension ref="A1:BC26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="S3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="U19" sqref="U19"/>
+      <selection pane="bottomRight" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" thickBottom="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" style="50" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" style="53" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" style="51" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.109375" style="51" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="10.6640625" style="51" customWidth="1"/>
-    <col min="11" max="12" width="12.6640625" style="51" customWidth="1"/>
-    <col min="13" max="13" width="15.109375" style="51" bestFit="1" customWidth="1"/>
-    <col min="14" max="17" width="12.6640625" style="51" customWidth="1"/>
-    <col min="18" max="18" width="22.5546875" style="51" bestFit="1" customWidth="1"/>
-    <col min="19" max="24" width="10.6640625" style="51" customWidth="1"/>
-    <col min="25" max="25" width="17.33203125" style="51" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.88671875" style="51" bestFit="1" customWidth="1"/>
-    <col min="27" max="30" width="10.6640625" style="51" customWidth="1"/>
-    <col min="31" max="31" width="24.33203125" style="51" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="24.33203125" style="51" customWidth="1"/>
-    <col min="33" max="33" width="13.44140625" style="51" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="22.5546875" style="51" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="30.6640625" style="51" customWidth="1"/>
-    <col min="36" max="36" width="22.5546875" style="51" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="19.109375" style="63" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="19.109375" style="65" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" style="48" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" style="50" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" style="49" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.109375" style="49" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="10.6640625" style="49" customWidth="1"/>
+    <col min="11" max="12" width="12.6640625" style="49" customWidth="1"/>
+    <col min="13" max="13" width="15.109375" style="49" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="12.6640625" style="49" customWidth="1"/>
+    <col min="18" max="18" width="22.5546875" style="49" bestFit="1" customWidth="1"/>
+    <col min="19" max="24" width="10.6640625" style="49" customWidth="1"/>
+    <col min="25" max="25" width="17.33203125" style="49" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.88671875" style="49" bestFit="1" customWidth="1"/>
+    <col min="27" max="30" width="10.6640625" style="49" customWidth="1"/>
+    <col min="31" max="31" width="24.33203125" style="49" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="24.33203125" style="49" customWidth="1"/>
+    <col min="33" max="33" width="13.44140625" style="49" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="22.5546875" style="49" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="30.6640625" style="49" customWidth="1"/>
+    <col min="36" max="36" width="22.5546875" style="49" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="19.109375" style="59" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="19.109375" style="60" bestFit="1" customWidth="1"/>
     <col min="39" max="45" width="8.88671875" style="5"/>
     <col min="46" max="55" width="8.88671875" style="6"/>
     <col min="56" max="16384" width="8.88671875" style="1"/>
@@ -1750,44 +1786,44 @@
     <row r="1" spans="1:55" s="2" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
-      <c r="C1" s="82" t="s">
+      <c r="C1" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="82"/>
-      <c r="R1" s="82"/>
-      <c r="S1" s="82"/>
-      <c r="T1" s="82"/>
-      <c r="U1" s="82"/>
-      <c r="V1" s="82"/>
-      <c r="W1" s="82"/>
-      <c r="X1" s="82"/>
-      <c r="Y1" s="82"/>
-      <c r="Z1" s="82"/>
-      <c r="AA1" s="82"/>
-      <c r="AB1" s="82"/>
-      <c r="AC1" s="82"/>
-      <c r="AD1" s="82"/>
-      <c r="AE1" s="82"/>
-      <c r="AF1" s="82"/>
-      <c r="AG1" s="82"/>
-      <c r="AH1" s="82"/>
-      <c r="AI1" s="82"/>
-      <c r="AJ1" s="82"/>
-      <c r="AK1" s="82"/>
-      <c r="AL1" s="82"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="67"/>
+      <c r="R1" s="67"/>
+      <c r="S1" s="67"/>
+      <c r="T1" s="67"/>
+      <c r="U1" s="67"/>
+      <c r="V1" s="67"/>
+      <c r="W1" s="67"/>
+      <c r="X1" s="67"/>
+      <c r="Y1" s="67"/>
+      <c r="Z1" s="67"/>
+      <c r="AA1" s="67"/>
+      <c r="AB1" s="67"/>
+      <c r="AC1" s="67"/>
+      <c r="AD1" s="67"/>
+      <c r="AE1" s="67"/>
+      <c r="AF1" s="67"/>
+      <c r="AG1" s="67"/>
+      <c r="AH1" s="67"/>
+      <c r="AI1" s="67"/>
+      <c r="AJ1" s="67"/>
+      <c r="AK1" s="67"/>
+      <c r="AL1" s="67"/>
       <c r="AM1" s="4"/>
       <c r="AN1" s="4"/>
       <c r="AO1" s="4"/>
@@ -1851,143 +1887,143 @@
       <c r="BC2" s="7"/>
     </row>
     <row r="3" spans="1:55" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="93" t="s">
+      <c r="C3" s="78" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="85" t="s">
+      <c r="D3" s="70" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="95" t="s">
+      <c r="E3" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="95" t="s">
+      <c r="F3" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="92" t="s">
+      <c r="G3" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="92"/>
-      <c r="I3" s="92" t="s">
+      <c r="H3" s="77"/>
+      <c r="I3" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="92"/>
-      <c r="K3" s="78" t="s">
+      <c r="J3" s="77"/>
+      <c r="K3" s="88" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="79"/>
-      <c r="M3" s="79"/>
-      <c r="N3" s="79"/>
-      <c r="O3" s="79"/>
-      <c r="P3" s="79"/>
-      <c r="Q3" s="80"/>
-      <c r="R3" s="89" t="s">
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
+      <c r="O3" s="89"/>
+      <c r="P3" s="89"/>
+      <c r="Q3" s="90"/>
+      <c r="R3" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="S3" s="89"/>
-      <c r="T3" s="89"/>
-      <c r="U3" s="89"/>
-      <c r="V3" s="81" t="s">
+      <c r="S3" s="74"/>
+      <c r="T3" s="74"/>
+      <c r="U3" s="74"/>
+      <c r="V3" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="W3" s="81"/>
-      <c r="X3" s="81"/>
-      <c r="Y3" s="87" t="s">
+      <c r="W3" s="91"/>
+      <c r="X3" s="91"/>
+      <c r="Y3" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="Z3" s="87" t="s">
+      <c r="Z3" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="AA3" s="75" t="s">
+      <c r="AA3" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="AB3" s="75"/>
-      <c r="AC3" s="72" t="s">
+      <c r="AB3" s="85"/>
+      <c r="AC3" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="AD3" s="73"/>
-      <c r="AE3" s="73"/>
-      <c r="AF3" s="73"/>
-      <c r="AG3" s="73"/>
-      <c r="AH3" s="74"/>
-      <c r="AI3" s="76" t="s">
+      <c r="AD3" s="83"/>
+      <c r="AE3" s="83"/>
+      <c r="AF3" s="83"/>
+      <c r="AG3" s="83"/>
+      <c r="AH3" s="84"/>
+      <c r="AI3" s="86" t="s">
         <v>64</v>
       </c>
-      <c r="AJ3" s="76" t="s">
+      <c r="AJ3" s="86" t="s">
         <v>18</v>
       </c>
-      <c r="AK3" s="83" t="s">
+      <c r="AK3" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="AL3" s="90" t="s">
+      <c r="AL3" s="75" t="s">
         <v>19</v>
       </c>
       <c r="AP3" s="6"/>
     </row>
     <row r="4" spans="1:55" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="94"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
-      <c r="G4" s="67" t="s">
+      <c r="C4" s="79"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="67" t="s">
+      <c r="H4" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="67" t="s">
+      <c r="I4" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="67" t="s">
+      <c r="J4" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="68" t="s">
+      <c r="K4" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="L4" s="68" t="s">
+      <c r="L4" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="M4" s="68" t="s">
+      <c r="M4" s="63" t="s">
         <v>59</v>
       </c>
-      <c r="N4" s="68" t="s">
+      <c r="N4" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="O4" s="68" t="s">
+      <c r="O4" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="68" t="s">
+      <c r="P4" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="68" t="s">
+      <c r="Q4" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="R4" s="69" t="s">
+      <c r="R4" s="64" t="s">
         <v>60</v>
       </c>
-      <c r="S4" s="69" t="s">
+      <c r="S4" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="T4" s="69" t="s">
+      <c r="T4" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="U4" s="69" t="s">
+      <c r="U4" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="V4" s="70" t="s">
+      <c r="V4" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="W4" s="70" t="s">
+      <c r="W4" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="X4" s="70" t="s">
+      <c r="X4" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="Y4" s="88"/>
-      <c r="Z4" s="88"/>
-      <c r="AA4" s="66" t="s">
+      <c r="Y4" s="73"/>
+      <c r="Z4" s="73"/>
+      <c r="AA4" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="AB4" s="66" t="s">
+      <c r="AB4" s="61" t="s">
         <v>5</v>
       </c>
       <c r="AC4" s="47" t="s">
@@ -2008,55 +2044,60 @@
       <c r="AH4" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="AI4" s="77"/>
-      <c r="AJ4" s="77"/>
-      <c r="AK4" s="84"/>
-      <c r="AL4" s="91"/>
+      <c r="AI4" s="87"/>
+      <c r="AJ4" s="87"/>
+      <c r="AK4" s="69"/>
+      <c r="AL4" s="76"/>
     </row>
     <row r="5" spans="1:55" ht="14.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="48"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="49"/>
-      <c r="N5" s="49"/>
-      <c r="O5" s="49"/>
-      <c r="P5" s="49"/>
-      <c r="Q5" s="49"/>
-      <c r="R5" s="49"/>
-      <c r="S5" s="49"/>
-      <c r="T5" s="49"/>
-      <c r="U5" s="49"/>
-      <c r="V5" s="49"/>
-      <c r="W5" s="49"/>
-      <c r="X5" s="49"/>
-      <c r="Y5" s="49"/>
-      <c r="Z5" s="49"/>
-      <c r="AA5" s="49"/>
-      <c r="AB5" s="49"/>
-      <c r="AC5" s="49"/>
-      <c r="AD5" s="49"/>
-      <c r="AE5" s="49"/>
-      <c r="AF5" s="49"/>
-      <c r="AG5" s="49"/>
-      <c r="AH5" s="49"/>
-      <c r="AI5" s="49"/>
-      <c r="AJ5" s="49"/>
-      <c r="AK5" s="62"/>
-      <c r="AL5" s="64"/>
+      <c r="C5" s="115"/>
+      <c r="D5" s="116"/>
+      <c r="E5" s="117"/>
+      <c r="F5" s="117"/>
+      <c r="G5" s="117"/>
+      <c r="H5" s="117"/>
+      <c r="I5" s="120"/>
+      <c r="J5" s="120"/>
+      <c r="K5" s="117"/>
+      <c r="L5" s="117"/>
+      <c r="M5" s="117"/>
+      <c r="N5" s="120"/>
+      <c r="O5" s="117"/>
+      <c r="P5" s="120"/>
+      <c r="Q5" s="120"/>
+      <c r="R5" s="119"/>
+      <c r="S5" s="119"/>
+      <c r="T5" s="120"/>
+      <c r="U5" s="120"/>
+      <c r="V5" s="117"/>
+      <c r="W5" s="120"/>
+      <c r="X5" s="120"/>
+      <c r="Y5" s="120"/>
+      <c r="Z5" s="119"/>
+      <c r="AA5" s="119"/>
+      <c r="AB5" s="119"/>
+      <c r="AC5" s="119"/>
+      <c r="AD5" s="119"/>
+      <c r="AE5" s="119"/>
+      <c r="AF5" s="119"/>
+      <c r="AG5" s="119"/>
+      <c r="AH5" s="119"/>
+      <c r="AI5" s="121"/>
+      <c r="AJ5" s="121"/>
+      <c r="AK5" s="122"/>
+      <c r="AL5" s="123"/>
+    </row>
+    <row r="6" spans="1:55" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M6" s="118"/>
     </row>
     <row r="26" spans="34:35" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="AH26" s="53"/>
-      <c r="AI26" s="71"/>
+      <c r="AH26" s="50"/>
+      <c r="AI26" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="AI3:AI4"/>
     <mergeCell ref="C1:AL1"/>
     <mergeCell ref="AK3:AK4"/>
     <mergeCell ref="D3:D4"/>
@@ -2073,8 +2114,6 @@
     <mergeCell ref="AA3:AB3"/>
     <mergeCell ref="AJ3:AJ4"/>
     <mergeCell ref="K3:Q3"/>
-    <mergeCell ref="V3:X3"/>
-    <mergeCell ref="AI3:AI4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2111,64 +2150,64 @@
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="107" t="s">
+      <c r="B2" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="107"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
       <c r="H2" s="23"/>
-      <c r="I2" s="107" t="s">
+      <c r="I2" s="99" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="107"/>
-      <c r="K2" s="107"/>
-      <c r="L2" s="107"/>
-      <c r="M2" s="107"/>
-      <c r="N2" s="107"/>
-      <c r="O2" s="107"/>
-      <c r="P2" s="107"/>
-      <c r="Q2" s="107"/>
-      <c r="R2" s="107"/>
-      <c r="S2" s="107"/>
-      <c r="T2" s="107"/>
-      <c r="U2" s="107"/>
-      <c r="V2" s="107"/>
-      <c r="W2" s="107"/>
-      <c r="X2" s="107"/>
-      <c r="Y2" s="107"/>
-      <c r="Z2" s="107"/>
-      <c r="AA2" s="107"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
+      <c r="N2" s="99"/>
+      <c r="O2" s="99"/>
+      <c r="P2" s="99"/>
+      <c r="Q2" s="99"/>
+      <c r="R2" s="99"/>
+      <c r="S2" s="99"/>
+      <c r="T2" s="99"/>
+      <c r="U2" s="99"/>
+      <c r="V2" s="99"/>
+      <c r="W2" s="99"/>
+      <c r="X2" s="99"/>
+      <c r="Y2" s="99"/>
+      <c r="Z2" s="99"/>
+      <c r="AA2" s="99"/>
     </row>
     <row r="3" spans="1:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="107"/>
-      <c r="C3" s="107"/>
-      <c r="D3" s="107"/>
-      <c r="E3" s="107"/>
-      <c r="F3" s="107"/>
-      <c r="G3" s="107"/>
+      <c r="B3" s="99"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
       <c r="H3" s="23"/>
-      <c r="I3" s="107"/>
-      <c r="J3" s="107"/>
-      <c r="K3" s="107"/>
-      <c r="L3" s="107"/>
-      <c r="M3" s="107"/>
-      <c r="N3" s="107"/>
-      <c r="O3" s="107"/>
-      <c r="P3" s="107"/>
-      <c r="Q3" s="107"/>
-      <c r="R3" s="107"/>
-      <c r="S3" s="107"/>
-      <c r="T3" s="107"/>
-      <c r="U3" s="107"/>
-      <c r="V3" s="107"/>
-      <c r="W3" s="107"/>
-      <c r="X3" s="107"/>
-      <c r="Y3" s="107"/>
-      <c r="Z3" s="107"/>
-      <c r="AA3" s="107"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="99"/>
+      <c r="N3" s="99"/>
+      <c r="O3" s="99"/>
+      <c r="P3" s="99"/>
+      <c r="Q3" s="99"/>
+      <c r="R3" s="99"/>
+      <c r="S3" s="99"/>
+      <c r="T3" s="99"/>
+      <c r="U3" s="99"/>
+      <c r="V3" s="99"/>
+      <c r="W3" s="99"/>
+      <c r="X3" s="99"/>
+      <c r="Y3" s="99"/>
+      <c r="Z3" s="99"/>
+      <c r="AA3" s="99"/>
     </row>
     <row r="4" spans="1:27" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="10"/>
@@ -2205,50 +2244,50 @@
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
-      <c r="J5" s="111" t="s">
+      <c r="J5" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="K5" s="112"/>
-      <c r="L5" s="113"/>
+      <c r="K5" s="104"/>
+      <c r="L5" s="105"/>
       <c r="M5" s="14"/>
       <c r="N5" s="12"/>
-      <c r="O5" s="54" t="s">
+      <c r="O5" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="P5" s="55" t="s">
+      <c r="P5" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="Q5" s="56" t="s">
+      <c r="Q5" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="R5" s="57" t="s">
+      <c r="R5" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="S5" s="56" t="s">
+      <c r="S5" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="T5" s="57" t="s">
+      <c r="T5" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="U5" s="56" t="s">
+      <c r="U5" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="V5" s="57" t="s">
+      <c r="V5" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="W5" s="56" t="s">
+      <c r="W5" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="X5" s="57" t="s">
+      <c r="X5" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="Y5" s="56" t="s">
+      <c r="Y5" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="Z5" s="57" t="s">
+      <c r="Z5" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="AA5" s="58" t="s">
+      <c r="AA5" s="55" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2281,21 +2320,21 @@
       <c r="AA6" s="20"/>
     </row>
     <row r="7" spans="1:27" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="97" t="s">
+      <c r="B7" s="95" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="98"/>
-      <c r="D7" s="98"/>
-      <c r="E7" s="99"/>
-      <c r="F7" s="100"/>
+      <c r="C7" s="96"/>
+      <c r="D7" s="96"/>
+      <c r="E7" s="97"/>
+      <c r="F7" s="98"/>
       <c r="G7" s="24"/>
       <c r="I7" s="10"/>
-      <c r="J7" s="108" t="s">
+      <c r="J7" s="100" t="s">
         <v>25</v>
       </c>
-      <c r="K7" s="109"/>
-      <c r="L7" s="109"/>
-      <c r="M7" s="110"/>
+      <c r="K7" s="101"/>
+      <c r="L7" s="101"/>
+      <c r="M7" s="102"/>
       <c r="N7" s="15"/>
       <c r="O7" s="27"/>
       <c r="P7" s="28"/>
@@ -2312,21 +2351,21 @@
       <c r="AA7" s="32"/>
     </row>
     <row r="8" spans="1:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="104" t="s">
+      <c r="B8" s="106" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="105"/>
-      <c r="D8" s="105"/>
-      <c r="E8" s="106"/>
-      <c r="F8" s="100"/>
+      <c r="C8" s="107"/>
+      <c r="D8" s="107"/>
+      <c r="E8" s="108"/>
+      <c r="F8" s="98"/>
       <c r="G8" s="25"/>
       <c r="I8" s="10"/>
-      <c r="J8" s="59" t="s">
+      <c r="J8" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="K8" s="60"/>
-      <c r="L8" s="60"/>
-      <c r="M8" s="61"/>
+      <c r="K8" s="57"/>
+      <c r="L8" s="57"/>
+      <c r="M8" s="58"/>
       <c r="N8" s="16"/>
       <c r="O8" s="33"/>
       <c r="P8" s="34"/>
@@ -2343,21 +2382,21 @@
       <c r="AA8" s="38"/>
     </row>
     <row r="9" spans="1:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="104" t="s">
+      <c r="B9" s="106" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="105"/>
-      <c r="D9" s="105"/>
-      <c r="E9" s="106"/>
-      <c r="F9" s="100"/>
+      <c r="C9" s="107"/>
+      <c r="D9" s="107"/>
+      <c r="E9" s="108"/>
+      <c r="F9" s="98"/>
       <c r="G9" s="25"/>
       <c r="I9" s="10"/>
-      <c r="J9" s="59" t="s">
+      <c r="J9" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="K9" s="60"/>
-      <c r="L9" s="60"/>
-      <c r="M9" s="61"/>
+      <c r="K9" s="57"/>
+      <c r="L9" s="57"/>
+      <c r="M9" s="58"/>
       <c r="N9" s="17"/>
       <c r="O9" s="33"/>
       <c r="P9" s="34"/>
@@ -2374,21 +2413,21 @@
       <c r="AA9" s="38"/>
     </row>
     <row r="10" spans="1:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="104" t="s">
+      <c r="B10" s="106" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="105"/>
-      <c r="D10" s="105"/>
-      <c r="E10" s="106"/>
-      <c r="F10" s="100"/>
+      <c r="C10" s="107"/>
+      <c r="D10" s="107"/>
+      <c r="E10" s="108"/>
+      <c r="F10" s="98"/>
       <c r="G10" s="25"/>
       <c r="I10" s="10"/>
-      <c r="J10" s="114" t="s">
+      <c r="J10" s="109" t="s">
         <v>28</v>
       </c>
-      <c r="K10" s="115"/>
-      <c r="L10" s="115"/>
-      <c r="M10" s="116"/>
+      <c r="K10" s="110"/>
+      <c r="L10" s="110"/>
+      <c r="M10" s="111"/>
       <c r="N10" s="17"/>
       <c r="O10" s="33"/>
       <c r="P10" s="34"/>
@@ -2405,21 +2444,21 @@
       <c r="AA10" s="38"/>
     </row>
     <row r="11" spans="1:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="101" t="s">
+      <c r="B11" s="92" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="102"/>
-      <c r="D11" s="102"/>
-      <c r="E11" s="103"/>
-      <c r="F11" s="100"/>
+      <c r="C11" s="93"/>
+      <c r="D11" s="93"/>
+      <c r="E11" s="94"/>
+      <c r="F11" s="98"/>
       <c r="G11" s="26"/>
       <c r="I11" s="10"/>
-      <c r="J11" s="117" t="s">
+      <c r="J11" s="112" t="s">
         <v>29</v>
       </c>
-      <c r="K11" s="118"/>
-      <c r="L11" s="118"/>
-      <c r="M11" s="119"/>
+      <c r="K11" s="113"/>
+      <c r="L11" s="113"/>
+      <c r="M11" s="114"/>
       <c r="N11" s="21"/>
       <c r="O11" s="39"/>
       <c r="P11" s="40"/>
@@ -2465,22 +2504,22 @@
     </row>
     <row r="13" spans="1:27" s="7" customFormat="1" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
-      <c r="B13" s="97" t="s">
+      <c r="B13" s="95" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="98"/>
-      <c r="D13" s="98"/>
-      <c r="E13" s="99"/>
-      <c r="F13" s="100"/>
+      <c r="C13" s="96"/>
+      <c r="D13" s="96"/>
+      <c r="E13" s="97"/>
+      <c r="F13" s="98"/>
       <c r="G13" s="24"/>
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
-      <c r="J13" s="97" t="s">
+      <c r="J13" s="95" t="s">
         <v>30</v>
       </c>
-      <c r="K13" s="98"/>
-      <c r="L13" s="98"/>
-      <c r="M13" s="99"/>
+      <c r="K13" s="96"/>
+      <c r="L13" s="96"/>
+      <c r="M13" s="97"/>
       <c r="N13" s="22"/>
       <c r="O13" s="27"/>
       <c r="P13" s="28"/>
@@ -2498,22 +2537,22 @@
     </row>
     <row r="14" spans="1:27" s="7" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
-      <c r="B14" s="104" t="s">
+      <c r="B14" s="106" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="105"/>
-      <c r="D14" s="105"/>
-      <c r="E14" s="106"/>
-      <c r="F14" s="100"/>
+      <c r="C14" s="107"/>
+      <c r="D14" s="107"/>
+      <c r="E14" s="108"/>
+      <c r="F14" s="98"/>
       <c r="G14" s="25"/>
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
-      <c r="J14" s="104" t="s">
+      <c r="J14" s="106" t="s">
         <v>31</v>
       </c>
-      <c r="K14" s="105"/>
-      <c r="L14" s="105"/>
-      <c r="M14" s="106"/>
+      <c r="K14" s="107"/>
+      <c r="L14" s="107"/>
+      <c r="M14" s="108"/>
       <c r="N14" s="22"/>
       <c r="O14" s="33"/>
       <c r="P14" s="34"/>
@@ -2531,22 +2570,22 @@
     </row>
     <row r="15" spans="1:27" s="7" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
-      <c r="B15" s="101" t="s">
+      <c r="B15" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="102"/>
-      <c r="D15" s="102"/>
-      <c r="E15" s="103"/>
-      <c r="F15" s="100"/>
+      <c r="C15" s="93"/>
+      <c r="D15" s="93"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="98"/>
       <c r="G15" s="26"/>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
-      <c r="J15" s="101" t="s">
+      <c r="J15" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="K15" s="102"/>
-      <c r="L15" s="102"/>
-      <c r="M15" s="103"/>
+      <c r="K15" s="93"/>
+      <c r="L15" s="93"/>
+      <c r="M15" s="94"/>
       <c r="N15" s="22"/>
       <c r="O15" s="39"/>
       <c r="P15" s="40"/>
@@ -2591,22 +2630,22 @@
       <c r="AA16" s="46"/>
     </row>
     <row r="17" spans="2:27" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="97" t="s">
+      <c r="B17" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="98"/>
-      <c r="D17" s="98"/>
-      <c r="E17" s="99"/>
-      <c r="F17" s="100"/>
+      <c r="C17" s="96"/>
+      <c r="D17" s="96"/>
+      <c r="E17" s="97"/>
+      <c r="F17" s="98"/>
       <c r="G17" s="24"/>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
-      <c r="J17" s="97" t="s">
+      <c r="J17" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="K17" s="98"/>
-      <c r="L17" s="98"/>
-      <c r="M17" s="99"/>
+      <c r="K17" s="96"/>
+      <c r="L17" s="96"/>
+      <c r="M17" s="97"/>
       <c r="N17" s="15"/>
       <c r="O17" s="27"/>
       <c r="P17" s="28"/>
@@ -2623,22 +2662,22 @@
       <c r="AA17" s="32"/>
     </row>
     <row r="18" spans="2:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="101" t="s">
+      <c r="B18" s="92" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="102"/>
-      <c r="D18" s="102"/>
-      <c r="E18" s="103"/>
-      <c r="F18" s="100"/>
+      <c r="C18" s="93"/>
+      <c r="D18" s="93"/>
+      <c r="E18" s="94"/>
+      <c r="F18" s="98"/>
       <c r="G18" s="26"/>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
-      <c r="J18" s="101" t="s">
+      <c r="J18" s="92" t="s">
         <v>34</v>
       </c>
-      <c r="K18" s="102"/>
-      <c r="L18" s="102"/>
-      <c r="M18" s="103"/>
+      <c r="K18" s="93"/>
+      <c r="L18" s="93"/>
+      <c r="M18" s="94"/>
       <c r="N18" s="17"/>
       <c r="O18" s="39"/>
       <c r="P18" s="40"/>
@@ -2683,22 +2722,22 @@
       <c r="AA19" s="46"/>
     </row>
     <row r="20" spans="2:27" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="97" t="s">
+      <c r="B20" s="95" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="98"/>
-      <c r="D20" s="98"/>
-      <c r="E20" s="99"/>
-      <c r="F20" s="100"/>
+      <c r="C20" s="96"/>
+      <c r="D20" s="96"/>
+      <c r="E20" s="97"/>
+      <c r="F20" s="98"/>
       <c r="G20" s="24"/>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
-      <c r="J20" s="97" t="s">
+      <c r="J20" s="95" t="s">
         <v>52</v>
       </c>
-      <c r="K20" s="98"/>
-      <c r="L20" s="98"/>
-      <c r="M20" s="99"/>
+      <c r="K20" s="96"/>
+      <c r="L20" s="96"/>
+      <c r="M20" s="97"/>
       <c r="N20" s="15"/>
       <c r="O20" s="27"/>
       <c r="P20" s="28"/>
@@ -2715,22 +2754,22 @@
       <c r="AA20" s="32"/>
     </row>
     <row r="21" spans="2:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="101" t="s">
+      <c r="B21" s="92" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="102"/>
-      <c r="D21" s="102"/>
-      <c r="E21" s="103"/>
-      <c r="F21" s="100"/>
+      <c r="C21" s="93"/>
+      <c r="D21" s="93"/>
+      <c r="E21" s="94"/>
+      <c r="F21" s="98"/>
       <c r="G21" s="26"/>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
-      <c r="J21" s="101" t="s">
+      <c r="J21" s="92" t="s">
         <v>53</v>
       </c>
-      <c r="K21" s="102"/>
-      <c r="L21" s="102"/>
-      <c r="M21" s="103"/>
+      <c r="K21" s="93"/>
+      <c r="L21" s="93"/>
+      <c r="M21" s="94"/>
       <c r="N21" s="17"/>
       <c r="O21" s="39"/>
       <c r="P21" s="40"/>
@@ -2775,22 +2814,22 @@
       <c r="AA22" s="46"/>
     </row>
     <row r="23" spans="2:27" s="9" customFormat="1" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="97" t="s">
+      <c r="B23" s="95" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="98"/>
-      <c r="D23" s="98"/>
-      <c r="E23" s="99"/>
-      <c r="F23" s="100"/>
+      <c r="C23" s="96"/>
+      <c r="D23" s="96"/>
+      <c r="E23" s="97"/>
+      <c r="F23" s="98"/>
       <c r="G23" s="24"/>
       <c r="H23" s="10"/>
       <c r="I23" s="10"/>
-      <c r="J23" s="97" t="s">
+      <c r="J23" s="95" t="s">
         <v>52</v>
       </c>
-      <c r="K23" s="98"/>
-      <c r="L23" s="98"/>
-      <c r="M23" s="99"/>
+      <c r="K23" s="96"/>
+      <c r="L23" s="96"/>
+      <c r="M23" s="97"/>
       <c r="N23" s="15"/>
       <c r="O23" s="27"/>
       <c r="P23" s="28"/>
@@ -2807,22 +2846,22 @@
       <c r="AA23" s="32"/>
     </row>
     <row r="24" spans="2:27" s="9" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="101" t="s">
+      <c r="B24" s="92" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="102"/>
-      <c r="D24" s="102"/>
-      <c r="E24" s="103"/>
-      <c r="F24" s="100"/>
+      <c r="C24" s="93"/>
+      <c r="D24" s="93"/>
+      <c r="E24" s="94"/>
+      <c r="F24" s="98"/>
       <c r="G24" s="26"/>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
-      <c r="J24" s="101" t="s">
+      <c r="J24" s="92" t="s">
         <v>53</v>
       </c>
-      <c r="K24" s="102"/>
-      <c r="L24" s="102"/>
-      <c r="M24" s="103"/>
+      <c r="K24" s="93"/>
+      <c r="L24" s="93"/>
+      <c r="M24" s="94"/>
       <c r="N24" s="17"/>
       <c r="O24" s="39"/>
       <c r="P24" s="40"/>
@@ -2921,24 +2960,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="J21:M21"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="J23:M23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="J24:M24"/>
-    <mergeCell ref="I2:AA3"/>
-    <mergeCell ref="J7:M7"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="B2:G3"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F7:F11"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="J10:M10"/>
-    <mergeCell ref="J11:M11"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="F20:F21"/>
     <mergeCell ref="J20:M20"/>
@@ -2955,6 +2976,24 @@
     <mergeCell ref="J17:M17"/>
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="B21:E21"/>
+    <mergeCell ref="I2:AA3"/>
+    <mergeCell ref="J7:M7"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="B2:G3"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F7:F11"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="J10:M10"/>
+    <mergeCell ref="J11:M11"/>
+    <mergeCell ref="J21:M21"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="J24:M24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>